<commit_message>
excel good food actualise
</commit_message>
<xml_diff>
--- a/Accessibilité Good food.xlsx
+++ b/Accessibilité Good food.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Desktop\Stage Bruxelles Environnement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Desktop\Stage Bruxelles Environnement\Modales_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CB404A-92A8-4A39-987E-900B8E908992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D593C57F-D0A5-4529-952B-DC34297BA413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{24BD21B7-A2EC-4EFE-B40D-1CC638ABDC62}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{24BD21B7-A2EC-4EFE-B40D-1CC638ABDC62}"/>
   </bookViews>
   <sheets>
     <sheet name="Ressources" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
   <si>
     <t>Lien vers la page</t>
   </si>
@@ -379,6 +379,21 @@
   </si>
   <si>
     <t>Ou les "' voir plus " (ou bien utiliser un aria-label pour être plus précis.</t>
+  </si>
+  <si>
+    <t>CHANGEMENTS FAITS</t>
+  </si>
+  <si>
+    <t>niveau de titres, explicité liens (FR -Nl)</t>
+  </si>
+  <si>
+    <t>niveau de titres, explicité liens (même version en nl)</t>
+  </si>
+  <si>
+    <t>niveaux de titres, version française en nl mais j'ai du changer aussi dans la version nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">niveaux de titres et listes à puces (NL ET FR)  </t>
   </si>
 </sst>
 </file>
@@ -426,12 +441,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -453,7 +474,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -789,107 +812,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F40EC9D-08CF-4F6E-B540-DDD3116F7BD1}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65:B66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="45.77734375" customWidth="1"/>
-    <col min="2" max="2" width="72.77734375" customWidth="1"/>
+    <col min="2" max="2" width="100.5546875" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
@@ -1293,7 +1332,7 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1435,7 +1474,7 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+      <c r="A20" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1448,7 +1487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C30437B1-F7DA-4FD8-BC42-B11D31A7CE34}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="B12:C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
actus excel accessibilite Good Food
</commit_message>
<xml_diff>
--- a/Accessibilité Good food.xlsx
+++ b/Accessibilité Good food.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Desktop\Stage Bruxelles Environnement\Modales_BE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D593C57F-D0A5-4529-952B-DC34297BA413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D6045F-AE60-460C-9096-39F8287806E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{24BD21B7-A2EC-4EFE-B40D-1CC638ABDC62}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{24BD21B7-A2EC-4EFE-B40D-1CC638ABDC62}"/>
   </bookViews>
   <sheets>
     <sheet name="Ressources" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="159">
   <si>
     <t>Lien vers la page</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Explicité liens</t>
   </si>
   <si>
-    <t>les liens ici ne sont pas du tout explicite</t>
-  </si>
-  <si>
     <t xml:space="preserve">Trucs et astuces pour prendre soin de soi </t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t xml:space="preserve">Plutôt mettre " Cultivé, cuisiné, animé"  en niveau de titres </t>
   </si>
   <si>
-    <t>https://goodfood.benoitcollienne.com/fr/contributions/vert-diris-formation-en-entrepreneuriat-social-pour-lalimentation-durable?domain=cit</t>
-  </si>
-  <si>
     <t xml:space="preserve">Formation en entrepreunarriat social </t>
   </si>
   <si>
@@ -375,9 +369,6 @@
     <t xml:space="preserve">https://goodfood.benoitcollienne.com/fr/commerces/bonpain-boulangerie-et-patisserie-bio?domain=cit </t>
   </si>
   <si>
-    <t xml:space="preserve"> https://goodfood.benoitcollienne.com/fr/commerces/bos-coop-supermarkt-supermarche-participatif?domain=cit   </t>
-  </si>
-  <si>
     <t>Ou les "' voir plus " (ou bien utiliser un aria-label pour être plus précis.</t>
   </si>
   <si>
@@ -394,13 +385,169 @@
   </si>
   <si>
     <t xml:space="preserve">niveaux de titres et listes à puces (NL ET FR)  </t>
+  </si>
+  <si>
+    <t>niveau de titres, fr et nl (même version fr))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">espacements et intitulé site (fr et nl </t>
+  </si>
+  <si>
+    <t>liste à puces (fr &amp; nl)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajout d'un intitulé de lien - remarqué par après </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> titre niveau 2 ajouté fr et nl - dans version fr le titre qui est de niveau 2 maintenant est en gras mais pas forcémnt sur les auntrdes pages le laisser ainsi?</t>
+  </si>
+  <si>
+    <r>
+      <t>les liens ici ne sont pas du tout explicite -</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>où?</t>
+    </r>
+  </si>
+  <si>
+    <t>niveaux de titres fr et  texte fr dans version nl</t>
+  </si>
+  <si>
+    <t>niveaux de titres eet liste à  puces fr et version  fr dans nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liste  à puces  fr et version fr dans nl </t>
+  </si>
+  <si>
+    <t>niveaux de titres et explicité liens aussi en NL- vertsion fr  dans nl</t>
+  </si>
+  <si>
+    <t>niveaux de titres fr -même  version en nl</t>
+  </si>
+  <si>
+    <t>suppression des puces et mise en place de titres de niveau 2 en remplacement - même content en nl</t>
+  </si>
+  <si>
+    <t>niveaux de titres et explicité liens  (à véérifier)-même content en nl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://goodfood.benoitcollienne.com/fr/contributions/vert-diris-formation-en-entrepreneuriat-social-pour-lalimentation-durable?domain=cit </t>
+  </si>
+  <si>
+    <t>niveaux dee titres et liste  à puces -même content en nm</t>
+  </si>
+  <si>
+    <t>je sais pas si fait le changement,, c'est peut-être  plus logique comme c'est maintenant ??</t>
+  </si>
+  <si>
+    <t>niveaux de titres et explicité liens fr et nl ('même contenu qu'en français)</t>
+  </si>
+  <si>
+    <t>titres déjà  bien structurés mais explicité lien corrigé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">structures de titres + explicité lien nl et fr +  remplacement du "en" par le "et" pour les numéros de téléphone dans la version fr </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://goodfood.benoitcollienne.com/fr/commerces/bos-coop-supermarkt-supermarche-participatif?domain=cit </t>
+  </si>
+  <si>
+    <t>A toutes faims utiles</t>
+  </si>
+  <si>
+    <t>structures de titres + explicité lien nl et fr</t>
+  </si>
+  <si>
+    <t>ApeReif</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://goodfood.brussels/fr/commerces/toutes-faims-utiles-artisan-traiteur?domain=cit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://goodfood.brussels/fr/commerces/apereiff-srl?domain=cit  </t>
+  </si>
+  <si>
+    <t>structure de titres fr et nl</t>
+  </si>
+  <si>
+    <t>AquaponieBXL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://goodfood.brussels/fr/commerces/aquaponiebxl-potagers-aquaponiques?domain=cit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">explicité liens  fr et nl </t>
+  </si>
+  <si>
+    <t>Artfood traiteur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://goodfood.brussels/fr/commerces/artfood-traiteur?domain=cit </t>
+  </si>
+  <si>
+    <t>Au petit bio'nheur</t>
+  </si>
+  <si>
+    <t>explicité liens  fr et nl  et structure de  titres.  NB : par hasard j'ai vu  que le lien vers leur site web ne marchait pas . Serait ce  plutôt ce site : http://www.bionheur.org/page_inst_2.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.bionheur.org/page_inst_2.php  </t>
+  </si>
+  <si>
+    <t>Au rayon bio miroir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://goodfood.brussels/fr/commerces/au-rayon-bio-miroir-magasin-specialiste-du-vrac?domain=cit </t>
+  </si>
+  <si>
+    <t>structure titres et explicité liens</t>
+  </si>
+  <si>
+    <t>Autentic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://goodfood.brussels/fr/commerces/autentic-production-artisanale-de-sauces-bio-et-de-plats-mijotes?domain=cit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">explicité liens fr et nl </t>
+  </si>
+  <si>
+    <t>Babl Market</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://goodfood.brussels/fr/commerces/babl-market-supermarche-cooperatif-et-participatif?domain=cit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">explicités lienss fr ett nl </t>
+  </si>
+  <si>
+    <t>Babine</t>
+  </si>
+  <si>
+    <t>https://goodfood.brussels/fr/commerces/babine-box-de-bieres-artisanales-belges?domain=cit</t>
+  </si>
+  <si>
+    <t>explicité liens fr et nl- je me suis permis d'ajouter le contenu français dans nl étant donné qu'il y était pas. En effet, sur les autress  pages nl  où il y a pas de texte en nl, le texte en fr est quand même mis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bam! </t>
+  </si>
+  <si>
+    <t>https://goodfood.brussels/fr/commerces/bam-alimentation-zero-dechet?domain=cit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,6 +587,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -468,14 +622,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -814,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F40EC9D-08CF-4F6E-B540-DDD3116F7BD1}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,340 +997,433 @@
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>109</v>
+      <c r="B1" s="4"/>
+      <c r="C1" s="8" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>110</v>
+      <c r="B2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" t="s">
-        <v>111</v>
+      <c r="B6" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" t="s">
-        <v>112</v>
+      <c r="B9" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" s="2" t="s">
-        <v>82</v>
+      <c r="C14" s="4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
-        <v>83</v>
+      <c r="B15" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="1" t="s">
+      <c r="C16" s="4"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="4"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
+      <c r="C18" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="4"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
+      <c r="B21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="4"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B25" s="2" t="s">
+      <c r="C24" s="4"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="4"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B32" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="4"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
+      <c r="C34" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="4"/>
+    </row>
+    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="4"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B38" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="4"/>
+    </row>
+    <row r="39" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B39" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B32" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B39" s="2" t="s">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="C46" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B50" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C52" s="4"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B58" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B42" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B47" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B55" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B56" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>56</v>
-      </c>
-      <c r="B57" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B58" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B59" t="s">
-        <v>94</v>
-      </c>
+      <c r="C59" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1185,9 +1446,10 @@
     <hyperlink ref="B39" r:id="rId17" xr:uid="{9A0CF1E8-7A72-4C50-9914-927488E19690}"/>
     <hyperlink ref="B41" r:id="rId18" xr:uid="{9AD9D1F7-FD66-4E26-A549-14EDAD1F44B1}"/>
     <hyperlink ref="B46" r:id="rId19" xr:uid="{87C9E713-D316-42B4-9F7B-90B4C8EF3FAA}"/>
+    <hyperlink ref="B57" r:id="rId20" xr:uid="{9D0BFFAC-F14B-4347-9BFB-7608DEA83CFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
@@ -1196,7 +1458,7 @@
   <dimension ref="A2:C17"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E21" sqref="A19:E21"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1212,38 +1474,38 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1263,12 +1525,12 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -1288,102 +1550,254 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F3403A6-92CE-4DB6-A0BC-C48E7E6DFFF2}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:N7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="76.5546875" customWidth="1"/>
+    <col min="2" max="2" width="102.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>77</v>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B30" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>158</v>
+      </c>
+      <c r="B38" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1393,6 +1807,15 @@
     <hyperlink ref="A10" r:id="rId3" xr:uid="{84EEBD2F-D74B-4FCB-A550-A8A0337D9830}"/>
     <hyperlink ref="A11" r:id="rId4" xr:uid="{54907CD1-0F84-498B-8A37-DCD289BAF2EC}"/>
     <hyperlink ref="A13" r:id="rId5" xr:uid="{EB236434-50BF-46E3-80C8-8DBCB6DD406F}"/>
+    <hyperlink ref="A18" r:id="rId6" xr:uid="{F66ABF73-EC96-41DC-AD4B-D49640CDC09B}"/>
+    <hyperlink ref="A20" r:id="rId7" xr:uid="{C850CD6A-BE45-437A-8837-B769293512B7}"/>
+    <hyperlink ref="A22" r:id="rId8" xr:uid="{C7C16B78-AE59-4BD5-9607-F6CBBBF24037}"/>
+    <hyperlink ref="A24" r:id="rId9" xr:uid="{6210195F-2FEB-41E0-BC5A-30EF4B1A885F}"/>
+    <hyperlink ref="A26" r:id="rId10" xr:uid="{070C4153-924C-4884-BC18-A88C826F8911}"/>
+    <hyperlink ref="A28" r:id="rId11" xr:uid="{80D157B8-7012-4A86-A85D-972E59EE6E5E}"/>
+    <hyperlink ref="A30" r:id="rId12" xr:uid="{A56AF085-B778-46A9-8DA1-AA9A6521D400}"/>
+    <hyperlink ref="A32" r:id="rId13" xr:uid="{9A7CAA24-573D-43D4-A95A-C2A1B66ADAC3}"/>
+    <hyperlink ref="A34" r:id="rId14" xr:uid="{D22CC128-F2CB-44E6-A3D9-B947A3FE278C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1410,32 +1833,32 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1445,37 +1868,37 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1522,18 +1945,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="6.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>